<commit_message>
Updated data model reference files #28
</commit_message>
<xml_diff>
--- a/data-raw/RDBES Data Model VD SL.xlsx
+++ b/data-raw/RDBES Data Model VD SL.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC062AD-D667-4FF0-AF69-8669A3E7C015}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665FF0DF-D877-401F-A1C5-523736BCAF50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="131">
   <si>
     <t>Hide</t>
   </si>
@@ -188,9 +188,6 @@
     <t>VDlen</t>
   </si>
   <si>
-    <t>3-160</t>
-  </si>
-  <si>
     <t>Overall length in metres.</t>
   </si>
   <si>
@@ -212,18 +209,12 @@
     <t>VDpwr</t>
   </si>
   <si>
-    <t>4-8500</t>
-  </si>
-  <si>
     <t>power in kW, and not in a category because it is needed to calculating the kWdays.</t>
   </si>
   <si>
     <t>Engine power (kW)</t>
   </si>
   <si>
-    <t>1-2500</t>
-  </si>
-  <si>
     <t>Vessel size in tonnes</t>
   </si>
   <si>
@@ -344,33 +335,9 @@
     <t>VDpower</t>
   </si>
   <si>
-    <t>Decimal</t>
-  </si>
-  <si>
-    <t>ISO_3166</t>
-  </si>
-  <si>
-    <t>Harbour_LOCODE</t>
-  </si>
-  <si>
-    <t>EDMO</t>
-  </si>
-  <si>
     <t>Institute uploading the species list.</t>
   </si>
   <si>
-    <t>RS_CatchFraction</t>
-  </si>
-  <si>
-    <t>SpecWoRMS</t>
-  </si>
-  <si>
-    <t>RS_VesselLengthCategory</t>
-  </si>
-  <si>
-    <t>RS_VesselSizeUnit</t>
-  </si>
-  <si>
     <t>The reference from SS to the SL is throgh; Country, SpeciesListName, Year and CatchFraction</t>
   </si>
   <si>
@@ -410,7 +377,43 @@
     <t>The exact name of the species list, which each country have uploaded to the Species list SL file.</t>
   </si>
   <si>
-    <t>Ver 19.1</t>
+    <t>4-9000</t>
+  </si>
+  <si>
+    <t>1-10000</t>
+  </si>
+  <si>
+    <t>Year //vocab.ices.dk/?ref=362</t>
+  </si>
+  <si>
+    <t>ISO_3166 //vocab.ices.dk/?ref=337</t>
+  </si>
+  <si>
+    <t>Harbour_LOCODE //vocab.ices.dk/?ref=1652</t>
+  </si>
+  <si>
+    <t>VesselLengthClass //vocab.ices.dk/?ref=1725</t>
+  </si>
+  <si>
+    <t>VesselSizeUnit //vocab.ices.dk/?ref=1632</t>
+  </si>
+  <si>
+    <t>SpecWoRMS //vocab.ices.dk/?ref=365</t>
+  </si>
+  <si>
+    <t>CatchFraction //vocab.ices.dk/?ref=1611</t>
+  </si>
+  <si>
+    <t>EDMO //vocab.ices.dk/?ref=1398</t>
+  </si>
+  <si>
+    <t>Decimal(2)</t>
+  </si>
+  <si>
+    <t>3.00-160</t>
+  </si>
+  <si>
+    <t>Ver 1.19.3</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,6 +468,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -520,9 +529,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -533,6 +539,21 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,7 +840,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -827,7 +848,7 @@
     <col min="5" max="5" width="15.86328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.86328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.1328125" customWidth="1"/>
+    <col min="11" max="11" width="21.265625" style="19" customWidth="1"/>
     <col min="12" max="12" width="41.265625" customWidth="1"/>
     <col min="13" max="13" width="39.265625" customWidth="1"/>
   </cols>
@@ -846,7 +867,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>5</v>
@@ -864,7 +885,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>10</v>
@@ -882,7 +903,7 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>40</v>
@@ -902,7 +923,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>16</v>
@@ -943,35 +964,35 @@
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D4" s="7">
         <v>2</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
@@ -980,7 +1001,7 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D5" s="7">
         <v>3</v>
@@ -989,13 +1010,13 @@
         <v>25</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>15</v>
@@ -1004,34 +1025,34 @@
         <v>28</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D6" s="7">
         <v>4</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>20</v>
@@ -1043,13 +1064,13 @@
         <v>28</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="24" x14ac:dyDescent="0.45">
@@ -1078,13 +1099,13 @@
         <v>28</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="24" x14ac:dyDescent="0.45">
@@ -1113,10 +1134,10 @@
         <v>28</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="M8" s="7" t="s">
         <v>49</v>
@@ -1138,24 +1159,24 @@
       <c r="G9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>107</v>
+      <c r="H9" s="18" t="s">
+        <v>128</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="7" t="s">
-        <v>55</v>
+      <c r="J9" s="18" t="s">
+        <v>129</v>
       </c>
       <c r="K9" s="7"/>
       <c r="L9" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="35.65" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="24" x14ac:dyDescent="0.45">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1163,13 +1184,13 @@
         <v>8</v>
       </c>
       <c r="E10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>20</v>
@@ -1180,14 +1201,14 @@
       <c r="J10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K10" s="7" t="s">
-        <v>114</v>
+      <c r="K10" s="18" t="s">
+        <v>123</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="24" x14ac:dyDescent="0.45">
@@ -1198,13 +1219,13 @@
         <v>9</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>42</v>
@@ -1212,15 +1233,15 @@
       <c r="I11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="11" t="s">
-        <v>63</v>
+      <c r="J11" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
@@ -1231,13 +1252,13 @@
         <v>10</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>42</v>
@@ -1245,15 +1266,15 @@
       <c r="I12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J12" s="11" t="s">
-        <v>66</v>
+      <c r="J12" s="17" t="s">
+        <v>119</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="35.65" x14ac:dyDescent="0.45">
@@ -1264,13 +1285,13 @@
         <v>11</v>
       </c>
       <c r="E13" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>98</v>
-      </c>
       <c r="G13" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>20</v>
@@ -1282,18 +1303,18 @@
         <v>28</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1310,7 +1331,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1320,12 +1341,12 @@
     <col min="6" max="6" width="17.86328125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="9.1328125" style="2"/>
-    <col min="11" max="11" width="14.86328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.3984375" style="19" customWidth="1"/>
     <col min="12" max="12" width="42.1328125" style="2" customWidth="1"/>
     <col min="13" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1339,7 +1360,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1357,7 +1378,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
@@ -1375,10 +1396,10 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -1393,363 +1414,363 @@
         <v>15</v>
       </c>
       <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="K2" s="20"/>
       <c r="L2" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11">
         <v>1</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13" t="s">
+      <c r="J3" s="11"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12" t="s">
+    <row r="4" spans="1:13" ht="24" x14ac:dyDescent="0.45">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>2</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="M4" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="13" t="s">
+    </row>
+    <row r="5" spans="1:13" ht="24" x14ac:dyDescent="0.45">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="11">
+        <v>3</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="12" t="s">
+      <c r="G5" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J5" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="11">
+        <v>4</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="11">
+        <v>5</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="K4" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="L4" s="9" t="s">
+      <c r="L7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="24" x14ac:dyDescent="0.45">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="11">
+        <v>6</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K8" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="M4" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="12">
-        <v>3</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="12" t="s">
+      <c r="L8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="11">
+        <v>7</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12" t="s">
+      <c r="J9" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="24" x14ac:dyDescent="0.45">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="12">
-        <v>4</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="12" t="s">
+      <c r="D10" s="11">
+        <v>8</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="12">
-        <v>5</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="12">
-        <v>6</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="12">
-        <v>7</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="12">
-        <v>8</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>113</v>
+      <c r="J10" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="13" t="s">
+      <c r="M10" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A13" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
+      <c r="A13" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">

</xml_diff>